<commit_message>
Altualização do nome da estação da LASER
</commit_message>
<xml_diff>
--- a/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
+++ b/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
   <si>
     <t>FT</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>BR1CNRKRC10</t>
+  </si>
+  <si>
+    <t>BR1CNRKLASER</t>
   </si>
 </sst>
 </file>
@@ -649,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1003,7 +1006,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Adicão dos hostnames da estação de AUTO_OBA
</commit_message>
<xml_diff>
--- a/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
+++ b/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="99">
   <si>
     <t>FT</t>
   </si>
@@ -286,6 +286,36 @@
   </si>
   <si>
     <t>BR1CNRKLASER</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA01</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA02</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA03</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA04</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA05</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA06</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA07</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA08</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA09</t>
+  </si>
+  <si>
+    <t>M_AUTO_OBA10</t>
   </si>
 </sst>
 </file>
@@ -653,7 +683,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1119,7 +1149,7 @@
         <v>48</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>47</v>
@@ -1130,7 +1160,7 @@
         <v>49</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>47</v>
@@ -1141,7 +1171,7 @@
         <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>47</v>
@@ -1152,7 +1182,7 @@
         <v>51</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>47</v>
@@ -1163,7 +1193,7 @@
         <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>47</v>
@@ -1174,7 +1204,7 @@
         <v>53</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>47</v>
@@ -1185,7 +1215,7 @@
         <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>47</v>
@@ -1196,7 +1226,7 @@
         <v>55</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>47</v>
@@ -1207,7 +1237,7 @@
         <v>56</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>47</v>
@@ -1218,7 +1248,7 @@
         <v>57</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Add mensagem de station name não encontrada
</commit_message>
<xml_diff>
--- a/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
+++ b/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
@@ -165,9 +165,6 @@
     <t>AUTO_OBA</t>
   </si>
   <si>
-    <t>AUTO_OBA1</t>
-  </si>
-  <si>
     <t>AUTO_OBA2</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>M_AUTO_OBA10</t>
+  </si>
+  <si>
+    <t>BR1CNRKOBA1</t>
   </si>
 </sst>
 </file>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -706,7 +706,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>10</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>26</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>28</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>30</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>32</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>34</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>47</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>47</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>47</v>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>47</v>
@@ -1190,10 +1190,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>47</v>
@@ -1201,10 +1201,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>47</v>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>47</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>47</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>47</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Adição de Classes para modelo BAYSIDE e inicio do Modelo LAKEPORT
</commit_message>
<xml_diff>
--- a/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
+++ b/WebServerSFC/TableStationTest/HostnamesROKU.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="120">
   <si>
     <t>FT</t>
   </si>
@@ -316,6 +316,69 @@
   </si>
   <si>
     <t>BR1CNRKOBA02</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL1</t>
+  </si>
+  <si>
+    <t>M_CAL01</t>
+  </si>
+  <si>
+    <t>CAL</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL2</t>
+  </si>
+  <si>
+    <t>M_CAL02</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL3</t>
+  </si>
+  <si>
+    <t>M_CAL03</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL4</t>
+  </si>
+  <si>
+    <t>M_CAL04</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL5</t>
+  </si>
+  <si>
+    <t>M_CAL05</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL6</t>
+  </si>
+  <si>
+    <t>M_CAL06</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL7</t>
+  </si>
+  <si>
+    <t>M_CAL07</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL8</t>
+  </si>
+  <si>
+    <t>M_CAL08</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL9</t>
+  </si>
+  <si>
+    <t>M_CAL09</t>
+  </si>
+  <si>
+    <t>BR1CNRKPCAL10</t>
+  </si>
+  <si>
+    <t>M_CAL10</t>
   </si>
 </sst>
 </file>
@@ -680,17 +743,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -816,441 +879,551 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>